<commit_message>
docs: modify labels placement
</commit_message>
<xml_diff>
--- a/mugna/assets/sample_basis.xlsx
+++ b/mugna/assets/sample_basis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\repos\Mugna\mugna\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A77C7E-5465-40CE-95CF-B48D59A50779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0432F864-D1E6-4877-A5E7-9E34B009592B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
   <si>
     <t>Company Name</t>
   </si>
@@ -41,36 +41,6 @@
   </si>
   <si>
     <t>Total Deduction</t>
-  </si>
-  <si>
-    <t>Daily Hour Rate</t>
-  </si>
-  <si>
-    <t>Nightly Hour Rate</t>
-  </si>
-  <si>
-    <t>Holiday Rate</t>
-  </si>
-  <si>
-    <t>Overtine Rate</t>
-  </si>
-  <si>
-    <t>Holiday Worked</t>
-  </si>
-  <si>
-    <t>Overtime Hours</t>
-  </si>
-  <si>
-    <t>Daily Hour Worked</t>
-  </si>
-  <si>
-    <t>Nightly Hour Worked</t>
-  </si>
-  <si>
-    <t>Total Daily Hour Pay</t>
-  </si>
-  <si>
-    <t>Total Nightly Hour Pay</t>
   </si>
   <si>
     <t>Total Holiday Pay</t>
@@ -95,6 +65,27 @@
   </si>
   <si>
     <t>Period:</t>
+  </si>
+  <si>
+    <t>Day Shift Hourly Rate</t>
+  </si>
+  <si>
+    <t>Night Shift Hourly Rate</t>
+  </si>
+  <si>
+    <t>Holiday Hourly Rate</t>
+  </si>
+  <si>
+    <t>Hour(s)  Worked</t>
+  </si>
+  <si>
+    <t>Total Day Shift Pay</t>
+  </si>
+  <si>
+    <t>Total Night Shift Pay</t>
+  </si>
+  <si>
+    <t>Overtime Rate</t>
   </si>
 </sst>
 </file>
@@ -162,7 +153,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +172,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -536,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -553,9 +550,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -610,9 +604,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -715,16 +706,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -748,24 +733,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -777,6 +747,51 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -786,6 +801,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFF2CC"/>
       <color rgb="FF90C4E8"/>
     </mruColors>
   </colors>
@@ -1065,169 +1081,169 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0.85546875" style="23" customWidth="1"/>
-    <col min="2" max="3" width="22.7109375" style="23" customWidth="1"/>
-    <col min="4" max="4" width="0.85546875" style="23" customWidth="1"/>
-    <col min="5" max="6" width="22.7109375" style="23" customWidth="1"/>
-    <col min="7" max="7" width="0.85546875" style="23" customWidth="1"/>
-    <col min="8" max="9" width="22.7109375" style="23" customWidth="1"/>
-    <col min="10" max="12" width="0.85546875" style="23" customWidth="1"/>
-    <col min="13" max="14" width="22.7109375" style="23" customWidth="1"/>
-    <col min="15" max="15" width="0.85546875" style="23" customWidth="1"/>
-    <col min="16" max="17" width="22.7109375" style="23" customWidth="1"/>
-    <col min="18" max="18" width="0.85546875" style="23" customWidth="1"/>
-    <col min="19" max="20" width="22.7109375" style="23" customWidth="1"/>
-    <col min="21" max="22" width="0.85546875" style="23" customWidth="1"/>
-    <col min="23" max="48" width="9.140625" style="23" customWidth="1"/>
-    <col min="49" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="1" width="0.85546875" style="22" customWidth="1"/>
+    <col min="2" max="3" width="22.7109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="0.85546875" style="22" customWidth="1"/>
+    <col min="5" max="6" width="22.7109375" style="22" customWidth="1"/>
+    <col min="7" max="7" width="0.85546875" style="22" customWidth="1"/>
+    <col min="8" max="9" width="22.7109375" style="22" customWidth="1"/>
+    <col min="10" max="12" width="0.85546875" style="22" customWidth="1"/>
+    <col min="13" max="14" width="22.7109375" style="22" customWidth="1"/>
+    <col min="15" max="15" width="0.85546875" style="22" customWidth="1"/>
+    <col min="16" max="17" width="22.7109375" style="22" customWidth="1"/>
+    <col min="18" max="18" width="0.85546875" style="22" customWidth="1"/>
+    <col min="19" max="20" width="22.7109375" style="22" customWidth="1"/>
+    <col min="21" max="22" width="0.85546875" style="22" customWidth="1"/>
+    <col min="23" max="48" width="9.140625" style="22" customWidth="1"/>
+    <col min="49" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="10"/>
-    </row>
-    <row r="2" spans="1:22" s="24" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="32" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="9"/>
+    </row>
+    <row r="2" spans="1:22" s="23" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="32" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="12"/>
-    </row>
-    <row r="3" spans="1:22" s="24" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="12"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="11"/>
+    </row>
+    <row r="3" spans="1:22" s="23" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="11"/>
     </row>
     <row r="4" spans="1:22" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="44" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="55"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="44" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="53"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="80" t="s">
-        <v>24</v>
-      </c>
-      <c r="U4" s="55"/>
-      <c r="V4" s="14"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="53"/>
+      <c r="V4" s="13"/>
     </row>
     <row r="5" spans="1:22" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="49"/>
-      <c r="S5" s="49"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="14"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="13"/>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="38" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="25" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="3"/>
@@ -1236,15 +1252,15 @@
         <v>4</v>
       </c>
       <c r="I6" s="5"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="38" t="s">
+      <c r="J6" s="27"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="36" t="s">
         <v>2</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
-      <c r="P6" s="27" t="s">
+      <c r="P6" s="25" t="s">
         <v>3</v>
       </c>
       <c r="Q6" s="3"/>
@@ -1253,458 +1269,460 @@
         <v>4</v>
       </c>
       <c r="T6" s="5"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="14"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="13"/>
     </row>
     <row r="7" spans="1:22" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="52"/>
-      <c r="V7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="50"/>
+      <c r="V7" s="13"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="73"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="68"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="N8" s="68"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="57"/>
-      <c r="S8" s="57" t="s">
+      <c r="C8" s="64"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="67"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="64"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="T8" s="68"/>
-      <c r="U8" s="61"/>
-      <c r="V8" s="14"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="55"/>
+      <c r="S8" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="T8" s="64"/>
+      <c r="U8" s="58"/>
+      <c r="V8" s="13"/>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="65"/>
+      <c r="D9" s="75"/>
       <c r="E9" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27" t="s">
+      <c r="G9" s="84"/>
+      <c r="H9" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="65"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="69"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="N9" s="69"/>
+      <c r="N9" s="65"/>
       <c r="O9" s="3"/>
       <c r="P9" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="Q9" s="4"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="T9" s="69"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="14"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" s="65"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="13"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="73"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="68"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="N10" s="68"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="59" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="57"/>
-      <c r="S10" s="57" t="s">
+      <c r="C10" s="64"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="80"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="64"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="68"/>
-      <c r="U10" s="61"/>
-      <c r="V10" s="14"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="80"/>
+      <c r="R10" s="55"/>
+      <c r="S10" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="T10" s="64"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="13"/>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="66"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="70"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="70"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="51"/>
-      <c r="S11" s="51" t="s">
+      <c r="F11" s="18"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="66"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="66"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T11" s="70"/>
-      <c r="U11" s="52"/>
-      <c r="V11" s="14"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="T11" s="66"/>
+      <c r="U11" s="50"/>
+      <c r="V11" s="13"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="27"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="25"/>
       <c r="F12" s="3"/>
       <c r="G12" s="5"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="27"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="25"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="5"/>
-      <c r="U12" s="39"/>
-      <c r="V12" s="14"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="13"/>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="65" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="63" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="82"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="78" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="79"/>
+      <c r="J13" s="77"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="60" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="O13" s="17"/>
+      <c r="P13" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="82"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="78" t="s">
+        <v>11</v>
+      </c>
+      <c r="T13" s="79"/>
+      <c r="U13" s="59"/>
+      <c r="V13" s="13"/>
+    </row>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="71"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="I13" s="74"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" s="65" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" s="18"/>
-      <c r="P13" s="63" t="s">
+      <c r="F14" s="82"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="68"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="Q13" s="71"/>
-      <c r="R13" s="72"/>
-      <c r="S13" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="T13" s="74"/>
-      <c r="U13" s="62"/>
-      <c r="V13" s="14"/>
-    </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="66"/>
-      <c r="N14" s="77"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="75"/>
-      <c r="U14" s="39"/>
-      <c r="V14" s="14"/>
+      <c r="Q14" s="82"/>
+      <c r="R14" s="74"/>
+      <c r="S14" s="78"/>
+      <c r="T14" s="79"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="13"/>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="77"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="3"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="60" t="s">
-        <v>21</v>
-      </c>
+      <c r="E15" s="72"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="75"/>
       <c r="I15" s="76"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="66"/>
-      <c r="N15" s="77"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="68"/>
       <c r="O15" s="3"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="60" t="s">
-        <v>21</v>
-      </c>
+      <c r="P15" s="72"/>
+      <c r="Q15" s="73"/>
+      <c r="R15" s="74"/>
+      <c r="S15" s="75"/>
       <c r="T15" s="76"/>
-      <c r="U15" s="62"/>
-      <c r="V15" s="14"/>
+      <c r="U15" s="77"/>
+      <c r="V15" s="13"/>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="77"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="3"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="77"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="62"/>
+      <c r="N16" s="68"/>
       <c r="O16" s="3"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
-      <c r="U16" s="39"/>
-      <c r="V16" s="14"/>
+      <c r="U16" s="37"/>
+      <c r="V16" s="13"/>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="77"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="68"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="77"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="68"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
-      <c r="U17" s="39"/>
-      <c r="V17" s="14"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="13"/>
     </row>
     <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="78"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="69"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="27" t="s">
-        <v>22</v>
+      <c r="E18" s="25" t="s">
+        <v>12</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="I18" s="5"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="66"/>
-      <c r="N18" s="78"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="62"/>
+      <c r="N18" s="69"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="27" t="s">
-        <v>22</v>
+      <c r="P18" s="25" t="s">
+        <v>12</v>
       </c>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="T18" s="5"/>
-      <c r="U18" s="39"/>
-      <c r="V18" s="14"/>
+      <c r="U18" s="37"/>
+      <c r="V18" s="13"/>
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="66"/>
-      <c r="C19" s="78"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="69"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="66"/>
-      <c r="N19" s="78"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="62"/>
+      <c r="N19" s="69"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
       <c r="R19" s="5"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="39"/>
-      <c r="V19" s="14"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="13"/>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="79"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="70"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="67"/>
-      <c r="N20" s="79"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="70"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
-      <c r="U20" s="39"/>
-      <c r="V20" s="14"/>
+      <c r="U20" s="37"/>
+      <c r="V20" s="13"/>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="42"/>
-      <c r="S21" s="42"/>
-      <c r="T21" s="42"/>
-      <c r="U21" s="43"/>
-      <c r="V21" s="14"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="41"/>
+      <c r="V21" s="13"/>
     </row>
     <row r="22" spans="1:22" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="17"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="16"/>
     </row>
     <row r="23" spans="1:22" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -1729,7 +1747,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="22"/>
+      <c r="R24" s="21"/>
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2145,6 +2163,12 @@
       <c r="S44" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="T13:T14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>